<commit_message>
change availab if then and temaplates
</commit_message>
<xml_diff>
--- a/Projects/CCBZA/Data/Template_GROCERY.xlsx
+++ b/Projects/CCBZA/Data/Template_GROCERY.xlsx
@@ -21,6 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$16</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$S$16</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$S$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$S$16</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -520,9 +521,6 @@
     <t xml:space="preserve">Stills Category Cooler</t>
   </si>
   <si>
-    <t xml:space="preserve">KO PRODUCT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Check for each category - if there is not KO PRODUCT, then there should be 2 facing of KO PRODUCT in this category</t>
   </si>
   <si>
@@ -551,6 +549,9 @@
   </si>
   <si>
     <t xml:space="preserve">DOC Stills Availability of Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLETISER,JUST JUICE</t>
   </si>
 </sst>
 </file>
@@ -857,20 +858,20 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.1813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.2697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="1020" min="8" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.7953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.6232558139535"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1020" min="8" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,15 +1161,15 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,33 +1221,33 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.3116279069767"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="83.0651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.0232558139535"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="92.5441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="85.7720930232558"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="85.6511627906977"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="95.2511627906977"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,22 +1666,22 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.8418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.3162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="57.9627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,29 +2005,29 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4744186046512"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.2093023255814"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.26046511627907"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.3953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.2139534883721"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.1953488372093"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,22 +2387,22 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.3348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,33 +2483,33 @@
   </sheetPr>
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.5441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="103.986046511628"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="88.1116279069768"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.1627906976744"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.0604651162791"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.13953488372093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.7348837209302"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="84.4186046511628"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.5162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="77.7348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="90.8186046511628"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.1488372093023"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.7953488372093"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="86.8837209302326"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2925,13 +2926,13 @@
         <v>53</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>53</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="L11" s="13" t="n">
         <v>2</v>
@@ -2946,7 +2947,7 @@
         <v>11</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2954,7 +2955,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>160</v>
@@ -2963,22 +2964,22 @@
         <v>161</v>
       </c>
       <c r="E12" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>165</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>166</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>53</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="I12" s="13" t="s">
         <v>114</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L12" s="13" t="n">
         <v>2</v>
@@ -2993,7 +2994,7 @@
         <v>11</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3001,7 +3002,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>160</v>
@@ -3010,22 +3011,22 @@
         <v>161</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>53</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>53</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="L13" s="13" t="n">
         <v>2</v>
@@ -3040,7 +3041,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3048,7 +3049,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>160</v>
@@ -3066,13 +3067,13 @@
         <v>53</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>53</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="L14" s="13" t="n">
         <v>2</v>
@@ -3087,7 +3088,7 @@
         <v>11</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3095,7 +3096,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>160</v>
@@ -3113,13 +3114,13 @@
         <v>53</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>53</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="L15" s="13" t="n">
         <v>2</v>
@@ -3134,7 +3135,7 @@
         <v>11</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,7 +3143,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>160</v>
@@ -3160,13 +3161,13 @@
         <v>53</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="I16" s="13" t="s">
         <v>114</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="L16" s="13" t="n">
         <v>2</v>
@@ -3181,7 +3182,7 @@
         <v>11</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>